<commit_message>
Timesheet Updated by Gokulraj
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet 1 (2).xlsx
+++ b/Process/Timesheet/PTW-Timesheet 1 (2).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{65FE4778-CBF0-43A0-96D0-A21CEC3ECEF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F046C6B7-8E44-4739-A968-F1FC7225202C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="182">
   <si>
     <t>Resource Name</t>
   </si>
@@ -515,6 +515,12 @@
     <t xml:space="preserve">Training Head and Co-ordinator Dessign flow </t>
   </si>
   <si>
+    <t>Team Disscussion 20 mins about design flow, Worked on Training Head and co-ordinator design flow 120 mins, Meeting with client (Rafi) - 90mins, Team Discussion about Design and Entity - 20mins, Alteration in Head and Co-ordinator Design flow - 120mins</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lunch and Tea break-90min                         </t>
+  </si>
+  <si>
     <t xml:space="preserve"> Data model Relationship </t>
   </si>
   <si>
@@ -579,6 +585,12 @@
   </si>
   <si>
     <t>Entity Data model and its Relationship</t>
+  </si>
+  <si>
+    <t>Entity datamodel  for all users</t>
+  </si>
+  <si>
+    <t>Discussion with team -20min, meeting rafi -1.30hours , Entity data model for trainee and integrated with others-3 hours</t>
   </si>
   <si>
     <t xml:space="preserve">Reviewed acceptance criteria for Trainee, Trainer, Training co ordinator, Trainnig Head. </t>
@@ -2507,8 +2519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{996EE506-C210-4575-ABFA-32B522DBF415}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15"/>
@@ -2589,10 +2601,10 @@
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="14" t="s">
-        <v>97</v>
+        <v>153</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>98</v>
+        <v>154</v>
       </c>
       <c r="G4" s="12"/>
       <c r="H4" s="18"/>
@@ -2602,17 +2614,17 @@
         <v>17</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>96</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="14" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="13"/>
@@ -2622,17 +2634,17 @@
         <v>19</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>101</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="14" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G6" s="4"/>
     </row>
@@ -2641,17 +2653,17 @@
         <v>20</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D7" s="5"/>
-      <c r="E7" s="13" t="s">
-        <v>161</v>
+      <c r="E7" s="12" t="s">
+        <v>163</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G7" s="4"/>
     </row>
@@ -2660,17 +2672,17 @@
         <v>21</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="13" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G8" s="4"/>
     </row>
@@ -2679,17 +2691,17 @@
         <v>22</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="G9" s="4"/>
     </row>
@@ -2698,17 +2710,17 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="14" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G10" s="4"/>
     </row>
@@ -2717,20 +2729,18 @@
         <v>24</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>112</v>
+        <v>177</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>114</v>
-      </c>
+      <c r="E11" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="F11" s="12"/>
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:8" ht="87" customHeight="1">
@@ -2738,19 +2748,19 @@
         <v>86</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>116</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="G12" s="4"/>
     </row>

</xml_diff>